<commit_message>
adding averages and more checks
</commit_message>
<xml_diff>
--- a/Employee_Reports28/-.xlsx
+++ b/Employee_Reports28/-.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,10 +28,7 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <color rgb="00FFFFFF"/>
     </font>
   </fonts>
   <fills count="3">
@@ -71,7 +68,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>